<commit_message>
This code now completely working and debugged.
</commit_message>
<xml_diff>
--- a/ready_patents/LyondellBasell.xlsx
+++ b/ready_patents/LyondellBasell.xlsx
@@ -17,9 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
-  <si>
-    <t>Sector</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>Section</t>
   </si>
   <si>
     <t>Description</t>
@@ -58,10 +58,10 @@
     <t>Keywords in context</t>
   </si>
   <si>
-    <t>Полимерные компаунды, полимерные смеси</t>
-  </si>
-  <si>
-    <t>Патент описывает полимерную композицию, содержащую линейный полиэтилен малой плотности (LLDPE) и реакторный термопластический полимер (rTPO), используемую для изготовления мембран, листов и других изделий. Добавление LLDPE повышает стабильность формы изделий, не влияя на другие свойства композиции. Композиция может содержать наполнители и добавки в определенных пропорциях. Реакторный термопластический полимер может содержать гомополимер пропилена и/или кополимер пропилена с этиленом и альфа-олефинами, а также дополнительные компоненты.</t>
+    <t>Полимерные компаунды</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Данный патент описывает полимерную композицию на основе полиолефина, которая может использоваться для производства мембран и других изделий. Композиция содержит термопластичный полимер, произведенный в реакторе (rTPO) и по меньшей мере один линейный полиэтилен низкой плотности (LLDPE), что позволяет улучшить стабильность размеров и силу термического расширения по сравнению с композицией, содержащей только rTPO, без влияния на другие свойства. Композиция также может содержать пакет добавок и/или пакет наполнителей. </t>
   </si>
   <si>
     <t>US20220380584

</xml_diff>